<commit_message>
Adding a data_template sheet to the template with column names to use, without data
</commit_message>
<xml_diff>
--- a/inst/extdata/template.xlsx
+++ b/inst/extdata/template.xlsx
@@ -12,7 +12,8 @@
     <sheet name="parcelle" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="modalite" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="placette" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="dictionary" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="data_template" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="dictionary" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="essai.organization_name">'essai'!$A$2:$A$150</definedName>
@@ -41,6 +42,9 @@
     <definedName name="placette.plot_y">'placette'!$E$2:$E$150</definedName>
     <definedName name="placette.plot_n">'placette'!$F$2:$F$150</definedName>
     <definedName name="placette.plot_desc">'placette'!$G$2:$G$150</definedName>
+    <definedName name="data_template.observation_date">'data_template'!$A$2:$A$150</definedName>
+    <definedName name="data_template.bbch_stage">'data_template'!$B$2:$B$150</definedName>
+    <definedName name="data_template.plot_id">'data_template'!$C$2:$C$150</definedName>
   </definedNames>
 </workbook>
 </file>
@@ -449,6 +453,72 @@
 </comments>
 </file>
 
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" mc:Ignorable="xr">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <color rgb="FF000000"/>
+            <family val="2"/>
+            <name val="Aptos Narrow"/>
+            <scheme val="minor"/>
+            <sz val="11"/>
+          </rPr>
+          <t xml:space="preserve">Date de réalisation de l'observation.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <color rgb="FF000000"/>
+            <family val="2"/>
+            <name val="Aptos Narrow"/>
+            <scheme val="minor"/>
+            <sz val="11"/>
+          </rPr>
+          <t xml:space="preserve">Stade phénologique lors de la mesure (échelle BBCH)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <color rgb="FF000000"/>
+            <family val="2"/>
+            <name val="Aptos Narrow"/>
+            <scheme val="minor"/>
+            <sz val="11"/>
+          </rPr>
+          <t xml:space="preserve">Code de la parcelle unitaire (ou élémentaire) permettant son identification unique au sein de l'expérimentation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <color rgb="FF000000"/>
+            <family val="2"/>
+            <name val="Aptos Narrow"/>
+            <scheme val="minor"/>
+            <sz val="11"/>
+          </rPr>
+          <t xml:space="preserve">Ajouter une colonne par variable, en respectant les noms de la Vitis Ontology. Voir https://vignevin.github.io/methodo/</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="1">
@@ -553,8 +623,20 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" id="5" name="Table5" displayName="Table5" ref="A1:G29" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:G29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" id="5" name="Table5" displayName="Table5" ref="A1:C2" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:C2"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="observation_date"/>
+    <tableColumn id="2" name="bbch_stage"/>
+    <tableColumn id="3" name="plot_id"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" id="6" name="Table6" displayName="Table6" ref="A1:G28" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:G28"/>
   <tableColumns count="7">
     <tableColumn id="1" name="nom"/>
     <tableColumn id="2" name="description_fr"/>
@@ -11868,7 +11950,65 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" bestFit="1" customWidth="1" hidden="false" width="17.625"/>
+    <col min="2" max="2" bestFit="1" customWidth="1" hidden="false" width="11.625"/>
+    <col min="3" max="3" bestFit="1" customWidth="1" hidden="false" width="8.625"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>observation_date</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>bbch_stage</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>plot_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions gridLines="1" gridLinesSet="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <legacyDrawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
@@ -12432,12 +12572,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>observation_name</t>
+          <t>organization_name</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Nom de l'observation.</t>
+          <t>Nom de l'institution responsable de l'expérimentation</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -12462,19 +12602,19 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>vignevin:observation_name</t>
+          <t>vignevin:organization_name</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>organization_name</t>
+          <t>plant_spacing</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Nom de l'institution responsable de l'expérimentation</t>
+          <t>Ecartement entre les ceps de vigne sur le rang, en m</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -12489,29 +12629,29 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t/>
+          <t>m</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>character</t>
+          <t>numeric</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>vignevin:organization_name</t>
+          <t>vignevin:plant_spacing</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>plant_spacing</t>
+          <t>plot_block</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Ecartement entre les ceps de vigne sur le rang, en m</t>
+          <t>Code du boc sur la quelle est située l'unité expérimentale. Un bloc regroupe plusieurs unités expérimentales. Les blocs sont utilisés pour réduire la variabilité expérimentale et améliorer la précision des comparaisons entre les traitements.</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -12526,29 +12666,29 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>m</t>
+          <t/>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>numeric</t>
+          <t>character</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>vignevin:plant_spacing</t>
+          <t>vignevin:plot_block</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>plot_block</t>
+          <t>plot_desc</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Code du boc sur la quelle est située l'unité expérimentale. Un bloc regroupe plusieurs unités expérimentales. Les blocs sont utilisés pour réduire la variabilité expérimentale et améliorer la précision des comparaisons entre les traitements.</t>
+          <t>Description ou commentaire sur la placette</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -12573,19 +12713,19 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>vignevin:plot_block</t>
+          <t>vignevin:plot_desc</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>plot_desc</t>
+          <t>plot_id</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Description ou commentaire sur la placette</t>
+          <t>Code de la parcelle unitaire (ou élémentaire) permettant son identification unique au sein de l'expérimentation</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -12610,19 +12750,19 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>vignevin:plot_desc</t>
+          <t>vignevin:plot_id</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>plot_id</t>
+          <t>plot_n</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Code de la parcelle unitaire (ou élémentaire) permettant son identification unique au sein de l'expérimentation</t>
+          <t>Nombre de ceps dans la parcelle unitaire</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -12642,24 +12782,24 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>character</t>
+          <t>interger</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>vignevin:plot_id</t>
+          <t>vignevin:plot_n</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>plot_n</t>
+          <t>plot_x</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Nombre de ceps dans la parcelle unitaire</t>
+          <t>Position de la parcelle unitaire en coordonnées relatives x. Typiquement, cela peut être un numéro de rang.</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -12684,19 +12824,19 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>vignevin:plot_n</t>
+          <t>vignevin:plot_x</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>plot_x</t>
+          <t>plot_y</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Position de la parcelle unitaire en coordonnées relatives x. Typiquement, cela peut être un numéro de rang.</t>
+          <t>Position de la parcelle unitaire en coordonnées relatives y. Typiquement, cela peut être le numéro de la 1er souche de la placette à partir du début du rang.</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -12721,19 +12861,19 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>vignevin:plot_x</t>
+          <t>vignevin:plot_y</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>plot_y</t>
+          <t>row_spacing</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Position de la parcelle unitaire en coordonnées relatives y. Typiquement, cela peut être le numéro de la 1er souche de la placette à partir du début du rang.</t>
+          <t>Ecartement entre les rangs de vigne, en m</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -12748,29 +12888,29 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t/>
+          <t>m</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>interger</t>
+          <t>numeric</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>vignevin:plot_y</t>
+          <t>vignevin:row_spacing</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>row_spacing</t>
+          <t>suborganization_name</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Ecartement entre les rangs de vigne, en m</t>
+          <t>Unité (appartenant à une organisation plus large).</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -12785,29 +12925,29 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>m</t>
+          <t/>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>numeric</t>
+          <t>character</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>vignevin:row_spacing</t>
+          <t>vignevin:suborganization_name</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>suborganization_name</t>
+          <t>xp_trt_code</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Unité (appartenant à une organisation plus large).</t>
+          <t>Code de la modalité (traitement expérimental)</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -12832,19 +12972,19 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>vignevin:suborganization_name</t>
+          <t>vignevin:xp_trt_code</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>xp_trt_code</t>
+          <t>xp_trt_desc</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Code de la modalité (traitement expérimental)</t>
+          <t>Description et commentaires sur le traitement expérimental</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -12869,19 +13009,19 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>vignevin:xp_trt_code</t>
+          <t>vignevin:xp_trt_desc</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>xp_trt_desc</t>
+          <t>xp_trt_name</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Description et commentaires sur le traitement expérimental</t>
+          <t>Nom court de la modalité (traitement expérimental)</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -12905,43 +13045,6 @@
         </is>
       </c>
       <c r="G28" t="inlineStr">
-        <is>
-          <t>vignevin:xp_trt_desc</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>xp_trt_name</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>Nom court de la modalité (traitement expérimental)</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>character</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
         <is>
           <t>vignevin:xp_trt_name</t>
         </is>

</xml_diff>

<commit_message>
initialize version 1.0.0 of startbox
</commit_message>
<xml_diff>
--- a/inst/extdata/template.xlsx
+++ b/inst/extdata/template.xlsx
@@ -37,7 +37,7 @@
     <definedName name="modalite.xp_trt_desc">'modalite'!$C$2:$C$150</definedName>
     <definedName name="placette.plot_id">'placette'!$A$2:$A$150</definedName>
     <definedName name="placette.xp_trt_code">'placette'!$B$2:$B$150</definedName>
-    <definedName name="placette.plot_block">'placette'!$C$2:$C$150</definedName>
+    <definedName name="placette.block_code">'placette'!$C$2:$C$150</definedName>
     <definedName name="placette.plot_x">'placette'!$D$2:$D$150</definedName>
     <definedName name="placette.plot_y">'placette'!$E$2:$E$150</definedName>
     <definedName name="placette.plot_n">'placette'!$F$2:$F$150</definedName>
@@ -612,7 +612,7 @@
   <tableColumns count="7">
     <tableColumn id="1" name="plot_id"/>
     <tableColumn id="2" name="xp_trt_code"/>
-    <tableColumn id="3" name="plot_block"/>
+    <tableColumn id="3" name="block_code"/>
     <tableColumn id="4" name="plot_x"/>
     <tableColumn id="5" name="plot_y"/>
     <tableColumn id="6" name="plot_n"/>
@@ -11865,7 +11865,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>plot_block</t>
+          <t>block_code</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
@@ -12091,12 +12091,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>commune_insee_id</t>
+          <t>block_code</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Code INSEE de la commune (5 caractères alphanumériques)</t>
+          <t>Code du boc sur la quelle est située l'unité expérimentale. Un bloc regroupe plusieurs unités expérimentales. Les blocs sont utilisés pour réduire la variabilité expérimentale et améliorer la précision des comparaisons entre les traitements.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -12121,19 +12121,19 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>vignevin:commune_insee_id</t>
+          <t>vignevin:block_code</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>commune_name</t>
+          <t>commune_insee_id</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Nom de la commune sur laquelle se trouve la parcelle</t>
+          <t>Code INSEE de la commune (5 caractères alphanumériques)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -12158,19 +12158,19 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>vignevin:commune_name</t>
+          <t>vignevin:commune_insee_id</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>cultivar_name</t>
+          <t>commune_name</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Nom de la variété (et clone si connu) produisant les fruits. Format de type "Syrah N Cl300" ou "Grenache B". Utiliser la nomenclature de https://www.plantgrape.fr/fr</t>
+          <t>Nom de la commune sur laquelle se trouve la parcelle</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -12195,19 +12195,19 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>vignevin:cultivar_name</t>
+          <t>vignevin:commune_name</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>design_plan</t>
+          <t>cultivar_name</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Type de plan d'expérience</t>
+          <t>Nom de la variété (et clone si connu) produisant les fruits. Format de type "Syrah N Cl300" ou "Grenache B". Utiliser la nomenclature de https://www.plantgrape.fr/fr</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -12232,19 +12232,19 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>vignevin:design_plan</t>
+          <t>vignevin:cultivar_name</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>email</t>
+          <t>design_plan</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Email de la personne</t>
+          <t>Type de plan d'expérience</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -12269,19 +12269,19 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>vignevin:email</t>
+          <t>vignevin:design_plan</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>expe_desc</t>
+          <t>email</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Description de l’expérimentation et des objectifs poursuivis</t>
+          <t>Email de la personne</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -12306,19 +12306,19 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>vignevin:expe_desc</t>
+          <t>vignevin:email</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>expe_end_date</t>
+          <t>expe_desc</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Date de fin de l’expérimentation. Elle est exprimée au format AAAA-MM-JJ suivant la norme internationale ISO 8601.</t>
+          <t>Description de l’expérimentation et des objectifs poursuivis</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -12338,24 +12338,24 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>character</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>vignevin:expe_end_date</t>
+          <t>vignevin:expe_desc</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>expe_name</t>
+          <t>expe_end_date</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Nom (ou code) usuel de l’expérimentation</t>
+          <t>Date de fin de l’expérimentation. Elle est exprimée au format AAAA-MM-JJ suivant la norme internationale ISO 8601.</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -12375,24 +12375,24 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>character</t>
+          <t>date</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>vignevin:expe_name</t>
+          <t>vignevin:expe_end_date</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>expe_start_date</t>
+          <t>expe_name</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Date de début de l’expérimentation. Elle est exprimée au format AAAA-MM-JJ suivant la norme internationale ISO 8601.</t>
+          <t>Nom (ou code) usuel de l’expérimentation</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -12412,24 +12412,24 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>character</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>vignevin:expe_start_date</t>
+          <t>vignevin:expe_name</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>field_latitude</t>
+          <t>expe_start_date</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Latitude du centroïde de la parcelle  (degrés décimaux WGS84)</t>
+          <t>Date de début de l’expérimentation. Elle est exprimée au format AAAA-MM-JJ suivant la norme internationale ISO 8601.</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -12444,29 +12444,29 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>decimal degrees</t>
+          <t/>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>numeric</t>
+          <t>date</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>vignevin:field_latitude</t>
+          <t>vignevin:expe_start_date</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>field_longitude</t>
+          <t>field_latitude</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Longitude du centroïde de la parcelle (degrés décimaux WGS84)</t>
+          <t>Latitude du centroïde de la parcelle  (degrés décimaux WGS84)</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -12491,19 +12491,19 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>vignevin:field_longitude</t>
+          <t>vignevin:field_latitude</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>field_name</t>
+          <t>field_longitude</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Nom (ou code) de la parcelle sur laquelle l’expérimentation a lieu</t>
+          <t>Longitude du centroïde de la parcelle (degrés décimaux WGS84)</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -12518,29 +12518,29 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t/>
+          <t>decimal degrees</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>character</t>
+          <t>numeric</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>vignevin:field_name</t>
+          <t>vignevin:field_longitude</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>observation_date</t>
+          <t>field_name</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Date de réalisation de l'observation.</t>
+          <t>Nom (ou code) de la parcelle sur laquelle l’expérimentation a lieu</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -12560,24 +12560,24 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>character</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>vignevin:observation_date</t>
+          <t>vignevin:field_name</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>organization_name</t>
+          <t>observation_date</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Nom de l'institution responsable de l'expérimentation</t>
+          <t>Date de réalisation de l'observation.</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -12597,24 +12597,24 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>character</t>
+          <t>date</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>vignevin:organization_name</t>
+          <t>vignevin:observation_date</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>plant_spacing</t>
+          <t>organization_name</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Ecartement entre les ceps de vigne sur le rang, en m</t>
+          <t>Nom de l'institution responsable de l'expérimentation</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -12629,29 +12629,29 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>m</t>
+          <t/>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>numeric</t>
+          <t>character</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>vignevin:plant_spacing</t>
+          <t>vignevin:organization_name</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>plot_block</t>
+          <t>plant_spacing</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Code du boc sur la quelle est située l'unité expérimentale. Un bloc regroupe plusieurs unités expérimentales. Les blocs sont utilisés pour réduire la variabilité expérimentale et améliorer la précision des comparaisons entre les traitements.</t>
+          <t>Ecartement entre les ceps de vigne sur le rang, en m</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -12666,17 +12666,17 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t/>
+          <t>m</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>character</t>
+          <t>numeric</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>vignevin:plot_block</t>
+          <t>vignevin:plant_spacing</t>
         </is>
       </c>
     </row>

</xml_diff>